<commit_message>
alternative analysis + baseline maturing
</commit_message>
<xml_diff>
--- a/reports/Term-1 Report/KTDA_EE499.xlsx
+++ b/reports/Term-1 Report/KTDA_EE499.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engineering\Biomedical\2021 1st Semester\EE499\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engineering\Biomedical\2021 1st Semester\EE499\on-campus-delivery-robot\reports\Term-1 Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7989B56F-FA89-413D-85F9-A51E49392466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527751B7-4566-4502-B7EB-56ED9A73A870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{46968C25-7865-432C-8A55-184323314E60}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="28800" windowHeight="15435" xr2:uid="{46968C25-7865-432C-8A55-184323314E60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B582D42-5293-440E-9D20-3ED6A4F40632}">
   <dimension ref="B2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" activeCellId="2" sqref="F2 G2 H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>